<commit_message>
complete working sp for cart
</commit_message>
<xml_diff>
--- a/data/game-data.xlsx
+++ b/data/game-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisa/Documents/OneDrive - UW Office 365/info-430/project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCC45BF-7AB4-EB49-A21B-28048245B91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6876FCB5-10C7-854E-87A0-0B28E3D1DCAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{02CB76CD-17B1-9441-809C-D6A55B88F13C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="90">
   <si>
     <t>GameReleaseDate</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>Playstation</t>
-  </si>
-  <si>
-    <t>Mobile</t>
   </si>
   <si>
     <t>Wii U</t>
@@ -669,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36858BE6-3422-4A47-B16E-F2BA71BFCA48}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,6 +779,15 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1367,7 +1373,7 @@
         <v>54</v>
       </c>
       <c r="G26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1468,7 +1474,7 @@
         <v>16</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H30" t="s">
         <v>86</v>

</xml_diff>